<commit_message>
fixed the unsaved changes in the RAG_sercher.ipynb file and added a function to load the FAISS index and documents.
</commit_message>
<xml_diff>
--- a/rag_results_log.xlsx
+++ b/rag_results_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,16 @@
           <t>chunk_overlap</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>chunking_strategy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-24 02:50:08</t>
+          <t>2025-07-24 14:51:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,17 +501,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>義大醫院醫研部誠徵碩士級研究技術員</t>
+          <t>國立中山大學新海研3號貴重儀器使用中心誠徵專任技術員1名</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/a0478e68-0991-42a7-a7d6-3779880333f8?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/ddc2e921-92c5-4004-8c2f-be2373c53f52?l=ch</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>具有組織染色相關訓練</t>
+          <t>相關應徵資料予以保密，合者約談，不合者恕不另行通知。 發佈日期：2025-07-04 00:00:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -520,11 +525,12 @@
       <c r="I2" t="n">
         <v>30</v>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-24 02:50:08</t>
+          <t>2025-07-24 14:51:24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -537,17 +543,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>【國立中央大學 應用地質研究所】誠徵 理工背景 研究計畫助理</t>
+          <t>[徵才] 國立臺灣大學防災減害與韌性學程 (綠‧韌性研究室) 徵求都市規劃/景觀/地理資訊專長 [專任計畫助理]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/f6f55778-1464-471e-8d9b-454b628ae816?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2793c7ef-b68d-4f00-9388-e011b78b9553?l=ch</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>無相關經驗可，具有學習意願</t>
+          <t>3.其他有利申請之相關文件 發佈日期：2025-07-21 00:00:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -561,11 +567,12 @@
       <c r="I3" t="n">
         <v>30</v>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-24 02:50:08</t>
+          <t>2025-07-24 14:51:24</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -578,17 +585,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>【誠徵博士後研究員】臺北醫學大學代謝與肥胖科學研究所林雅婷老師實驗室</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 博士後研究員</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/b9acd095-8dde-4fe5-91c1-d91b1cebc8b0?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/701ca4f1-a9f5-4a61-9b66-c4cf60f5c093?l=ch</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>有參考性相關資料</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -602,11 +609,12 @@
       <c r="I4" t="n">
         <v>30</v>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-24 02:50:08</t>
+          <t>2025-07-24 14:51:24</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -619,17 +627,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>高雄榮總教研部生殖暨粒線體醫學研究室---誠徵博士後研究員</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 碩士級研究助理</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/47729f59-955a-4b43-addd-5a18d1affa86?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2521ae27-55c0-4f27-9ded-b4bc908c1aff?l=ch</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>具有細胞及動物等相關研究經驗尤佳。</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -643,11 +651,12 @@
       <c r="I5" t="n">
         <v>30</v>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-24 02:50:08</t>
+          <t>2025-07-24 14:51:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -660,17 +669,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>國家衛生研究院神經及精神醫學研究中心劉翰璇助研究員誠徵研究助理1名</t>
+          <t>國立臺東大學通識教育中心徵聘專任助理教授以上教師徵才公告，收件至114年8月15日止。</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/945b153d-9c19-4730-8bec-abfd53bec0cd?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e407fdbc-62c9-4e09-b08a-35a897cc4186?l=ch</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>其它有助於審查之相關資料</t>
+          <t>其    它： 相關訊息，請至本校首頁徵人啟事https://psn.nttu.edu.tw/p/406-1047-165359,r595.php?Lang=zh-tw查詢下載。 聯絡人姓名: 李家婕小姐 聯絡人電話: 089-517492 電子信箱：evalee@nttu.edu.tw 發佈日期：2025-07-09 00:00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -684,11 +693,12 @@
       <c r="I6" t="n">
         <v>30</v>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:18</t>
+          <t>2025-07-24 15:35:07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -701,17 +711,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>義大醫院醫研部誠徵碩士級研究技術員</t>
+          <t>國立中山大學新海研3號貴重儀器使用中心誠徵專任技術員1名</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/a0478e68-0991-42a7-a7d6-3779880333f8?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/ddc2e921-92c5-4004-8c2f-be2373c53f52?l=ch</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>具有組織染色相關訓練</t>
+          <t>相關應徵資料予以保密，合者約談，不合者恕不另行通知。 發佈日期：2025-07-04 00:00:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -724,12 +734,17 @@
       </c>
       <c r="I7" t="n">
         <v>30</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:18</t>
+          <t>2025-07-24 15:35:07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -742,17 +757,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>【國立中央大學 應用地質研究所】誠徵 理工背景 研究計畫助理</t>
+          <t>[徵才] 國立臺灣大學防災減害與韌性學程 (綠‧韌性研究室) 徵求都市規劃/景觀/地理資訊專長 [專任計畫助理]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/f6f55778-1464-471e-8d9b-454b628ae816?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2793c7ef-b68d-4f00-9388-e011b78b9553?l=ch</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>無相關經驗可，具有學習意願</t>
+          <t>3.其他有利申請之相關文件 發佈日期：2025-07-21 00:00:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -765,12 +780,17 @@
       </c>
       <c r="I8" t="n">
         <v>30</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:18</t>
+          <t>2025-07-24 15:35:07</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -783,17 +803,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>【誠徵博士後研究員】臺北醫學大學代謝與肥胖科學研究所林雅婷老師實驗室</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 博士後研究員</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/b9acd095-8dde-4fe5-91c1-d91b1cebc8b0?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/701ca4f1-a9f5-4a61-9b66-c4cf60f5c093?l=ch</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>有參考性相關資料</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -806,12 +826,17 @@
       </c>
       <c r="I9" t="n">
         <v>30</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:18</t>
+          <t>2025-07-24 15:35:07</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -824,17 +849,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>高雄榮總教研部生殖暨粒線體醫學研究室---誠徵博士後研究員</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 碩士級研究助理</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/47729f59-955a-4b43-addd-5a18d1affa86?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2521ae27-55c0-4f27-9ded-b4bc908c1aff?l=ch</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>具有細胞及動物等相關研究經驗尤佳。</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -847,12 +872,17 @@
       </c>
       <c r="I10" t="n">
         <v>30</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:18</t>
+          <t>2025-07-24 15:35:07</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -865,17 +895,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>國家衛生研究院神經及精神醫學研究中心劉翰璇助研究員誠徵研究助理1名</t>
+          <t>國立臺東大學通識教育中心徵聘專任助理教授以上教師徵才公告，收件至114年8月15日止。</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/945b153d-9c19-4730-8bec-abfd53bec0cd?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e407fdbc-62c9-4e09-b08a-35a897cc4186?l=ch</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>其它有助於審查之相關資料</t>
+          <t>其    它： 相關訊息，請至本校首頁徵人啟事https://psn.nttu.edu.tw/p/406-1047-165359,r595.php?Lang=zh-tw查詢下載。 聯絡人姓名: 李家婕小姐 聯絡人電話: 089-517492 電子信箱：evalee@nttu.edu.tw 發佈日期：2025-07-09 00:00:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -888,17 +918,22 @@
       </c>
       <c r="I11" t="n">
         <v>30</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:44</t>
+          <t>2025-07-24 15:35:39</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>生物相關的職缺有哪些？</t>
+          <t>材料相關的職缺有哪些？</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -906,17 +941,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>高雄榮總教研部生殖暨粒線體醫學研究室---誠徵博士後研究員</t>
+          <t>國立中山大學新海研3號貴重儀器使用中心誠徵專任技術員1名</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/47729f59-955a-4b43-addd-5a18d1affa86?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/ddc2e921-92c5-4004-8c2f-be2373c53f52?l=ch</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>生物醫學相關領域畢業。</t>
+          <t>相關應徵資料予以保密，合者約談，不合者恕不另行通知。 發佈日期：2025-07-04 00:00:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -929,17 +964,22 @@
       </c>
       <c r="I12" t="n">
         <v>30</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:44</t>
+          <t>2025-07-24 15:35:39</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>生物相關的職缺有哪些？</t>
+          <t>材料相關的職缺有哪些？</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -947,17 +987,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>中國醫藥大學生物醫學研究所誠徵博士後研究員</t>
+          <t>[徵才] 國立臺灣大學防災減害與韌性學程 (綠‧韌性研究室) 徵求都市規劃/景觀/地理資訊專長 [專任計畫助理]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/cc8706e2-836d-4f85-94d2-89396360a823?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2793c7ef-b68d-4f00-9388-e011b78b9553?l=ch</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>生物醫學相關</t>
+          <t>3.其他有利申請之相關文件 發佈日期：2025-07-21 00:00:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -970,17 +1010,22 @@
       </c>
       <c r="I13" t="n">
         <v>30</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:44</t>
+          <t>2025-07-24 15:35:39</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>生物相關的職缺有哪些？</t>
+          <t>材料相關的職缺有哪些？</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -988,17 +1033,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>馬偕紀念醫院血液腫瘤科蘇迺文醫師誠徵國科會補助計畫專任助理</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 博士後研究員</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/a78b7d93-b5b4-4bb9-bff5-5888b2d695e6?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/701ca4f1-a9f5-4a61-9b66-c4cf60f5c093?l=ch</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>生命科學相關系所</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1011,17 +1056,22 @@
       </c>
       <c r="I14" t="n">
         <v>30</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:44</t>
+          <t>2025-07-24 15:35:39</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>生物相關的職缺有哪些？</t>
+          <t>材料相關的職缺有哪些？</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1029,17 +1079,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>台大醫院耳鼻喉部楊宗霖教授徵博士後研究員</t>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 碩士級研究助理</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/e2f4f22d-3604-4ce0-854e-94b9a0ce8c10?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2521ae27-55c0-4f27-9ded-b4bc908c1aff?l=ch</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>細胞生物相關技術</t>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1052,17 +1102,22 @@
       </c>
       <c r="I15" t="n">
         <v>30</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-07-24 02:56:44</t>
+          <t>2025-07-24 15:35:39</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>生物相關的職缺有哪些？</t>
+          <t>材料相關的職缺有哪些？</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1070,17 +1125,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>國家衛生研究院癌症研究所 誠徵院內博士後研究員或研究助理一名</t>
+          <t>國立臺東大學通識教育中心徵聘專任助理教授以上教師徵才公告，收件至114年8月15日止。</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.nstc.gov.tw/folksonomy/detail/95244417-fdb2-451f-812c-315ae9e234c4?l=ch</t>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e407fdbc-62c9-4e09-b08a-35a897cc4186?l=ch</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>具有生化、細胞、分生背景及細胞培養等相關研究經驗。</t>
+          <t>其    它： 相關訊息，請至本校首頁徵人啟事https://psn.nttu.edu.tw/p/406-1047-165359,r595.php?Lang=zh-tw查詢下載。 聯絡人姓名: 李家婕小姐 聯絡人電話: 089-517492 電子信箱：evalee@nttu.edu.tw 發佈日期：2025-07-09 00:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1093,6 +1148,11 @@
       </c>
       <c r="I16" t="n">
         <v>30</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add hybrid chunking and recursive chunking methods sentence_chunking_recursive and paragraph_chunking_recursive methods and their corresponding FAISS index and documents
</commit_message>
<xml_diff>
--- a/rag_results_log.xlsx
+++ b/rag_results_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1155,6 +1155,926 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-07-24 15:42:11</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>國立中山大學新海研3號貴重儀器使用中心誠徵專任技術員1名</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/ddc2e921-92c5-4004-8c2f-be2373c53f52?l=ch</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>相關應徵資料予以保密，合者約談，不合者恕不另行通知。 發佈日期：2025-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>300</v>
+      </c>
+      <c r="I17" t="n">
+        <v>30</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-07-24 15:42:11</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>[徵才] 國立臺灣大學防災減害與韌性學程 (綠‧韌性研究室) 徵求都市規劃/景觀/地理資訊專長 [專任計畫助理]</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2793c7ef-b68d-4f00-9388-e011b78b9553?l=ch</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3.其他有利申請之相關文件 發佈日期：2025-07-21 00:00:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>300</v>
+      </c>
+      <c r="I18" t="n">
+        <v>30</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-07-24 15:42:11</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 博士後研究員</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/701ca4f1-a9f5-4a61-9b66-c4cf60f5c093?l=ch</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>300</v>
+      </c>
+      <c r="I19" t="n">
+        <v>30</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-07-24 15:42:11</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 碩士級研究助理</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2521ae27-55c0-4f27-9ded-b4bc908c1aff?l=ch</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>300</v>
+      </c>
+      <c r="I20" t="n">
+        <v>30</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-07-24 15:42:11</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>國立臺東大學通識教育中心徵聘專任助理教授以上教師徵才公告，收件至114年8月15日止。</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e407fdbc-62c9-4e09-b08a-35a897cc4186?l=ch</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>其    它： 相關訊息，請至本校首頁徵人啟事https://psn.nttu.edu.tw/p/406-1047-165359,r595.php?Lang=zh-tw查詢下載。 聯絡人姓名: 李家婕小姐 聯絡人電話: 089-517492 電子信箱：evalee@nttu.edu.tw 發佈日期：2025-07-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>300</v>
+      </c>
+      <c r="I21" t="n">
+        <v>30</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:04:57</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>國立中山大學新海研3號貴重儀器使用中心誠徵專任技術員1名</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/ddc2e921-92c5-4004-8c2f-be2373c53f52?l=ch</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>相關應徵資料予以保密，合者約談，不合者恕不另行通知。 發佈日期：2025-07-04 00:00:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>300</v>
+      </c>
+      <c r="I22" t="n">
+        <v>30</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:04:57</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>[徵才] 國立臺灣大學防災減害與韌性學程 (綠‧韌性研究室) 徵求都市規劃/景觀/地理資訊專長 [專任計畫助理]</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2793c7ef-b68d-4f00-9388-e011b78b9553?l=ch</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>3.其他有利申請之相關文件 發佈日期：2025-07-21 00:00:00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>300</v>
+      </c>
+      <c r="I23" t="n">
+        <v>30</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:04:57</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 博士後研究員</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/701ca4f1-a9f5-4a61-9b66-c4cf60f5c093?l=ch</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>300</v>
+      </c>
+      <c r="I24" t="n">
+        <v>30</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:04:57</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>中國醫藥大學 癌症生物精準醫學研究中心  王紹椿老師實驗室 誠徵 碩士級研究助理</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/2521ae27-55c0-4f27-9ded-b4bc908c1aff?l=ch</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>歡迎對癌症研究有興趣的夥伴加入我們的團隊！ 發佈日期：2025-07-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>300</v>
+      </c>
+      <c r="I25" t="n">
+        <v>30</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:04:57</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>材料相關的職缺有哪些？</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>國立臺東大學通識教育中心徵聘專任助理教授以上教師徵才公告，收件至114年8月15日止。</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e407fdbc-62c9-4e09-b08a-35a897cc4186?l=ch</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>其    它： 相關訊息，請至本校首頁徵人啟事https://psn.nttu.edu.tw/p/406-1047-165359,r595.php?Lang=zh-tw查詢下載。 聯絡人姓名: 李家婕小姐 聯絡人電話: 089-517492 電子信箱：evalee@nttu.edu.tw 發佈日期：2025-07-09 00:00:00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>300</v>
+      </c>
+      <c r="I26" t="n">
+        <v>30</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:05:29</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>中國醫藥大學生物醫學研究所誠徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/cc8706e2-836d-4f85-94d2-89396360a823?l=ch</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>生物醫學相關</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>300</v>
+      </c>
+      <c r="I27" t="n">
+        <v>30</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:05:29</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>馬偕紀念醫院血液腫瘤科蘇迺文醫師誠徵國科會補助計畫專任助理</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/a78b7d93-b5b4-4bb9-bff5-5888b2d695e6?l=ch</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>生命科學相關系所</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>300</v>
+      </c>
+      <c r="I28" t="n">
+        <v>30</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:05:29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>高雄榮總教研部生殖暨粒線體醫學研究室---誠徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/47729f59-955a-4b43-addd-5a18d1affa86?l=ch</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>生物醫學相關領域畢業。</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>300</v>
+      </c>
+      <c r="I29" t="n">
+        <v>30</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:05:29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>台大醫院耳鼻喉部楊宗霖教授徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e2f4f22d-3604-4ce0-854e-94b9a0ce8c10?l=ch</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>細胞生物相關技術</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>300</v>
+      </c>
+      <c r="I30" t="n">
+        <v>30</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:05:29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>5</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>國家衛生研究院癌症研究所 誠徵院內博士後研究員或研究助理一名</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/95244417-fdb2-451f-812c-315ae9e234c4?l=ch</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>具有生化、細胞、分生背景及細胞培養等相關研究經驗。</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>300</v>
+      </c>
+      <c r="I31" t="n">
+        <v>30</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:07:59</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>中國醫藥大學生物醫學研究所誠徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/cc8706e2-836d-4f85-94d2-89396360a823?l=ch</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>生物醫學相關</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>300</v>
+      </c>
+      <c r="I32" t="n">
+        <v>30</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:07:59</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>馬偕紀念醫院血液腫瘤科蘇迺文醫師誠徵國科會補助計畫專任助理</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/a78b7d93-b5b4-4bb9-bff5-5888b2d695e6?l=ch</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>生命科學相關系所</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>300</v>
+      </c>
+      <c r="I33" t="n">
+        <v>30</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:07:59</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>3</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>高雄榮總教研部生殖暨粒線體醫學研究室---誠徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/47729f59-955a-4b43-addd-5a18d1affa86?l=ch</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>生物醫學相關領域畢業。</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>300</v>
+      </c>
+      <c r="I34" t="n">
+        <v>30</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:07:59</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>台大醫院耳鼻喉部楊宗霖教授徵博士後研究員</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/e2f4f22d-3604-4ce0-854e-94b9a0ce8c10?l=ch</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>細胞生物相關技術</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>300</v>
+      </c>
+      <c r="I35" t="n">
+        <v>30</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-07-24 16:07:59</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>生物相關的職缺有哪些</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>5</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>國家衛生研究院癌症研究所 誠徵院內博士後研究員或研究助理一名</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://www.nstc.gov.tw/folksonomy/detail/95244417-fdb2-451f-812c-315ae9e234c4?l=ch</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>具有生化、細胞、分生背景及細胞培養等相關研究經驗。</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>all-MiniLM-L6-v2</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>300</v>
+      </c>
+      <c r="I36" t="n">
+        <v>30</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>hybrid_chunking</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>